<commit_message>
added base.html and destination ems
</commit_message>
<xml_diff>
--- a/calc/files/ems_points.xlsx
+++ b/calc/files/ems_points.xlsx
@@ -12,6 +12,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a15="http://schemas.microsoft.com/office/drawing/2012/main" xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:co="http://ncloudtech.com" xmlns:co-ooxml="http://ncloudtech.com/ooxml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:x="urn:schemas-microsoft-com:office:excel" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="co co-ooxml w14 x14 w15">
   <si>
+    <r>
+      <rPr>
+        <rFont val="Roboto"/>
+        <b val="true"/>
+        <i val="false"/>
+        <color rgb="31353B" tint="0"/>
+        <sz val="9"/>
+      </rPr>
+      <t>Минск</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Roboto"/>
+        <b val="true"/>
+        <i val="false"/>
+        <color rgb="31353B" tint="0"/>
+        <sz val="9"/>
+      </rPr>
+      <t>Р6</t>
+    </r>
+  </si>
+  <si>
     <t>Барановичи Брестская обл.</t>
   </si>
   <si>
@@ -373,30 +397,6 @@
   </si>
   <si>
     <t>Малорита Брестская обл.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Roboto"/>
-        <b val="true"/>
-        <i val="false"/>
-        <color rgb="31353B" tint="0"/>
-        <sz val="9"/>
-      </rPr>
-      <t>Минск</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Roboto"/>
-        <b val="true"/>
-        <i val="false"/>
-        <color rgb="31353B" tint="0"/>
-        <sz val="9"/>
-      </rPr>
-      <t>Р6</t>
-    </r>
   </si>
   <si>
     <t>Минский район</t>
@@ -666,16 +666,16 @@
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" borderId="1" fillId="2" fontId="2" quotePrefix="false">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" borderId="1" fillId="2" fontId="3" quotePrefix="false">
+      <alignment horizontal="left" indent="1" vertical="top"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" borderId="1" fillId="2" fontId="3" quotePrefix="false">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" borderId="1" fillId="2" fontId="2" quotePrefix="false">
       <alignment horizontal="left" indent="1" vertical="top"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" borderId="1" fillId="2" fontId="2" quotePrefix="false">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" borderId="1" fillId="2" fontId="3" quotePrefix="false">
-      <alignment horizontal="left" indent="1" vertical="top"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" borderId="1" fillId="2" fontId="3" quotePrefix="false">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -923,10 +923,10 @@
       <c r="A2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -934,10 +934,10 @@
       <c r="A3" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -945,10 +945,10 @@
       <c r="A4" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -956,10 +956,10 @@
       <c r="A5" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -967,10 +967,10 @@
       <c r="A6" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -978,10 +978,10 @@
       <c r="A7" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -989,10 +989,10 @@
       <c r="A8" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1000,32 +1000,32 @@
       <c r="A9" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
+      <c r="C9" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>18</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1042,7 +1042,7 @@
     </row>
     <row outlineLevel="0" r="13">
       <c r="A13" s="2" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>23</v>
@@ -1053,139 +1053,139 @@
     </row>
     <row outlineLevel="0" r="14">
       <c r="A14" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>3</v>
+      <c r="C14" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row outlineLevel="0" r="15">
       <c r="A15" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="16">
       <c r="A16" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>13</v>
+      <c r="C16" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row outlineLevel="0" r="17">
       <c r="A17" s="2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="18">
       <c r="A18" s="2" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row outlineLevel="0" r="19">
       <c r="A19" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row outlineLevel="0" r="20">
       <c r="A20" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="21">
       <c r="A21" s="2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row outlineLevel="0" r="22">
       <c r="A22" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>36</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="23">
       <c r="A23" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>5</v>
+      <c r="C23" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row outlineLevel="0" r="24">
       <c r="A24" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row outlineLevel="0" r="25">
       <c r="A25" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>40</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row outlineLevel="0" r="26">
       <c r="A26" s="2" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>41</v>
@@ -1196,40 +1196,40 @@
     </row>
     <row outlineLevel="0" r="27">
       <c r="A27" s="2" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row outlineLevel="0" r="28">
       <c r="A28" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="29">
       <c r="A29" s="2" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row outlineLevel="0" r="30">
       <c r="A30" s="2" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>47</v>
@@ -1240,464 +1240,464 @@
     </row>
     <row outlineLevel="0" r="31">
       <c r="A31" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="B31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>3</v>
+      <c r="C31" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row outlineLevel="0" r="32">
       <c r="A32" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>7</v>
+        <v>32</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="33">
       <c r="A33" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="34">
       <c r="A34" s="2" t="n">
-        <v>35</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="35">
       <c r="A35" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>3</v>
+        <v>35</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row outlineLevel="0" r="36">
       <c r="A36" s="2" t="n">
-        <v>37</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>55</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="37">
       <c r="A37" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="B37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row outlineLevel="0" r="38">
       <c r="A38" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="B38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>36</v>
+      <c r="C38" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row outlineLevel="0" r="39">
       <c r="A39" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row outlineLevel="0" r="40">
       <c r="A40" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row outlineLevel="0" r="41">
       <c r="A41" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>18</v>
+        <v>41</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row outlineLevel="0" r="42">
       <c r="A42" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>13</v>
+        <v>42</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row outlineLevel="0" r="43">
       <c r="A43" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>7</v>
+        <v>43</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="44">
       <c r="A44" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="45">
       <c r="A45" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row outlineLevel="0" r="46">
       <c r="A46" s="2" t="n">
-        <v>47</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>5</v>
+        <v>46</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row outlineLevel="0" r="47">
       <c r="A47" s="2" t="n">
-        <v>48</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row outlineLevel="0" r="48">
       <c r="A48" s="2" t="n">
-        <v>49</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C48" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row outlineLevel="0" r="49">
       <c r="A49" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="B49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>24</v>
+      <c r="C49" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row outlineLevel="0" r="50">
       <c r="A50" s="2" t="n">
-        <v>51</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>40</v>
+        <v>50</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row outlineLevel="0" r="51">
       <c r="A51" s="2" t="n">
-        <v>52</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row outlineLevel="0" r="52">
       <c r="A52" s="2" t="n">
-        <v>53</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>74</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="53">
       <c r="A53" s="2" t="n">
-        <v>54</v>
-      </c>
-      <c r="B53" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>40</v>
+      <c r="C53" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row outlineLevel="0" r="54">
       <c r="A54" s="2" t="n">
-        <v>55</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>77</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row outlineLevel="0" r="55">
       <c r="A55" s="2" t="n">
-        <v>56</v>
-      </c>
-      <c r="B55" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>7</v>
+      <c r="C55" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row outlineLevel="0" r="56">
       <c r="A56" s="2" t="n">
-        <v>57</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>36</v>
+        <v>56</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="57">
       <c r="A57" s="2" t="n">
         <v>57</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>74</v>
+      <c r="B57" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row outlineLevel="0" r="58">
       <c r="A58" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>74</v>
+      <c r="B58" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row outlineLevel="0" r="59">
       <c r="A59" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>3</v>
+      <c r="B59" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row outlineLevel="0" r="60">
       <c r="A60" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>13</v>
+      <c r="B60" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="61">
       <c r="A61" s="2" t="n">
         <v>61</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>3</v>
+      <c r="B61" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="62">
       <c r="A62" s="2" t="n">
         <v>62</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>7</v>
+      <c r="B62" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="63">
       <c r="A63" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>18</v>
+      <c r="B63" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="64">
       <c r="A64" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>27</v>
+      <c r="B64" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row outlineLevel="0" r="65">
       <c r="A65" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C65" s="4" t="s">
+      <c r="B65" s="5" t="s">
         <v>89</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row outlineLevel="0" r="66">
       <c r="A66" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>11</v>
+      <c r="C66" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row outlineLevel="0" r="67">
       <c r="A67" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>7</v>
+      <c r="B67" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row outlineLevel="0" r="68">
       <c r="A68" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>13</v>
+      <c r="B68" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="69">
       <c r="A69" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>55</v>
+      <c r="B69" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="70">
       <c r="A70" s="2" t="n">
         <v>70</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>7</v>
+      <c r="B70" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row outlineLevel="0" r="71">
       <c r="A71" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>5</v>
+      <c r="B71" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="72">
       <c r="A72" s="2" t="n">
         <v>72</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>24</v>
+      <c r="B72" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row outlineLevel="0" r="73">
@@ -1705,42 +1705,42 @@
         <v>73</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
     </row>
     <row outlineLevel="0" r="74">
       <c r="A74" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>7</v>
+      <c r="C74" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="75">
       <c r="A75" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>27</v>
+      <c r="C75" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row outlineLevel="0" r="76">
       <c r="A76" s="2" t="n">
         <v>76</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C76" s="4" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1748,109 +1748,109 @@
       <c r="A77" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>3</v>
+      <c r="C77" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="78">
       <c r="A78" s="2" t="n">
         <v>78</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>69</v>
+      <c r="C78" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row outlineLevel="0" r="79">
       <c r="A79" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>7</v>
+      <c r="C79" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="80">
       <c r="A80" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>9</v>
+      <c r="C80" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row outlineLevel="0" r="81">
       <c r="A81" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C81" s="4" t="s">
-        <v>74</v>
+      <c r="C81" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row outlineLevel="0" r="82">
       <c r="A82" s="2" t="n">
         <v>82</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C82" s="4" t="s">
-        <v>7</v>
+      <c r="C82" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="83">
       <c r="A83" s="2" t="n">
         <v>83</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C83" s="4" t="s">
-        <v>18</v>
+      <c r="C83" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row outlineLevel="0" r="84">
       <c r="A84" s="2" t="n">
         <v>84</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C84" s="4" t="s">
-        <v>7</v>
+      <c r="C84" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="85">
       <c r="A85" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>36</v>
+      <c r="C85" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row outlineLevel="0" r="86">
       <c r="A86" s="2" t="n">
         <v>86</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="6" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1858,21 +1858,21 @@
       <c r="A87" s="2" t="n">
         <v>87</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>13</v>
+      <c r="C87" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="88">
       <c r="A88" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C88" s="6" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1880,21 +1880,21 @@
       <c r="A89" s="2" t="n">
         <v>89</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>15</v>
+      <c r="C89" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row outlineLevel="0" r="90">
       <c r="A90" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="6" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1902,10 +1902,10 @@
       <c r="A91" s="2" t="n">
         <v>91</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="6" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1913,21 +1913,21 @@
       <c r="A92" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C92" s="4" t="s">
-        <v>18</v>
+      <c r="C92" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row outlineLevel="0" r="93">
       <c r="A93" s="2" t="n">
         <v>93</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C93" s="6" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1935,10 +1935,10 @@
       <c r="A94" s="2" t="n">
         <v>94</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="6" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1946,142 +1946,142 @@
       <c r="A95" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C95" s="4" t="s">
-        <v>20</v>
+      <c r="C95" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row outlineLevel="0" r="96">
       <c r="A96" s="2" t="n">
         <v>96</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C96" s="4" t="s">
-        <v>24</v>
+      <c r="C96" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row outlineLevel="0" r="97">
       <c r="A97" s="2" t="n">
         <v>97</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C97" s="4" t="s">
-        <v>7</v>
+      <c r="C97" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="98">
       <c r="A98" s="2" t="n">
         <v>98</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C98" s="4" t="s">
-        <v>13</v>
+      <c r="C98" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="99">
       <c r="A99" s="2" t="n">
         <v>99</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C99" s="4" t="s">
-        <v>13</v>
+      <c r="C99" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="100">
       <c r="A100" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C100" s="4" t="s">
-        <v>27</v>
+      <c r="C100" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row outlineLevel="0" r="101">
       <c r="A101" s="2" t="n">
         <v>101</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>13</v>
+      <c r="C101" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="102">
       <c r="A102" s="2" t="n">
         <v>102</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C102" s="4" t="s">
-        <v>9</v>
+      <c r="C102" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row outlineLevel="0" r="103">
       <c r="A103" s="2" t="n">
         <v>103</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C103" s="4" t="s">
-        <v>57</v>
+      <c r="C103" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row outlineLevel="0" r="104">
       <c r="A104" s="2" t="n">
         <v>104</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B104" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>3</v>
+      <c r="C104" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="105">
       <c r="A105" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C105" s="4" t="s">
-        <v>9</v>
+      <c r="C105" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row outlineLevel="0" r="106">
       <c r="A106" s="2" t="n">
         <v>106</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C106" s="4" t="s">
-        <v>7</v>
+      <c r="C106" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="107">
       <c r="A107" s="2" t="n">
         <v>107</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B107" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C107" s="6" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2089,209 +2089,209 @@
       <c r="A108" s="2" t="n">
         <v>108</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C108" s="4" t="s">
-        <v>7</v>
+      <c r="C108" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="109">
       <c r="A109" s="2" t="n">
         <v>109</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C109" s="4" t="s">
-        <v>7</v>
+      <c r="C109" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="110">
       <c r="A110" s="2" t="n">
         <v>110</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C110" s="4" t="s">
-        <v>7</v>
+      <c r="C110" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="111">
       <c r="A111" s="2" t="n">
         <v>111</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C111" s="4" t="s">
-        <v>7</v>
+      <c r="C111" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="112">
       <c r="A112" s="2" t="n">
         <v>112</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C112" s="4" t="s">
-        <v>55</v>
+      <c r="C112" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row outlineLevel="0" r="113">
       <c r="A113" s="2" t="n">
         <v>113</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C113" s="4" t="s">
-        <v>57</v>
+      <c r="C113" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row outlineLevel="0" r="114">
       <c r="A114" s="2" t="n">
         <v>114</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C114" s="4" t="s">
-        <v>7</v>
+      <c r="C114" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="115">
       <c r="A115" s="2" t="n">
         <v>115</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C115" s="4" t="s">
-        <v>27</v>
+      <c r="C115" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row outlineLevel="0" r="116">
       <c r="A116" s="2" t="n">
         <v>116</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C116" s="4" t="s">
-        <v>18</v>
+      <c r="C116" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row outlineLevel="0" r="117">
       <c r="A117" s="2" t="n">
         <v>117</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C117" s="4" t="s">
-        <v>74</v>
+      <c r="C117" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row outlineLevel="0" r="118">
       <c r="A118" s="2" t="n">
         <v>118</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C118" s="4" t="s">
-        <v>3</v>
+      <c r="C118" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="119">
       <c r="A119" s="2" t="n">
         <v>119</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C119" s="4" t="s">
-        <v>27</v>
+      <c r="C119" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row outlineLevel="0" r="120">
       <c r="A120" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C120" s="4" t="s">
-        <v>7</v>
+      <c r="C120" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row outlineLevel="0" r="121">
       <c r="A121" s="2" t="n">
         <v>121</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C121" s="4" t="s">
-        <v>3</v>
+      <c r="C121" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="122">
       <c r="A122" s="2" t="n">
         <v>122</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C122" s="4" t="s">
-        <v>13</v>
+      <c r="C122" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="123">
       <c r="A123" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C123" s="4" t="s">
-        <v>20</v>
+      <c r="C123" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row outlineLevel="0" r="124">
       <c r="A124" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B124" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C124" s="4" t="s">
-        <v>3</v>
+      <c r="C124" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="125">
       <c r="A125" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B125" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C125" s="4" t="s">
-        <v>11</v>
+      <c r="C125" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row outlineLevel="0" r="126">
       <c r="A126" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B126" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C126" s="4" t="s">
-        <v>36</v>
+      <c r="C126" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>